<commit_message>
update Scenario4 Report script
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2376" windowWidth="9552" windowHeight="3564" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2376" windowWidth="9552" windowHeight="3564"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5231,8 +5231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5303,7 +5303,7 @@
         <v>160</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -5346,8 +5346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5458,10 +5458,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5580,11 +5580,6 @@
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated RTI scenario 4 upto Aug month
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3564" windowWidth="9552" xWindow="0" yWindow="2376"/>
+    <workbookView activeTab="18" firstSheet="15" windowHeight="3564" windowWidth="9552" xWindow="0" yWindow="2376"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="167">
   <si>
     <t>TC</t>
   </si>
@@ -282,9 +282,6 @@
     <t>TestAprilReports</t>
   </si>
   <si>
-    <t>F:\\Automation NI Reports\\HMRCTestData\\Payroll RTI Recognition Test Report 201718\\201718 Payroll RTI Recognition Test result.xlsx</t>
-  </si>
-  <si>
     <t>ProcessFinalPayrollForMay</t>
   </si>
   <si>
@@ -468,18 +465,6 @@
     <t>England</t>
   </si>
   <si>
-    <t>1000L</t>
-  </si>
-  <si>
-    <t>B Married women and widows entitled to pay reduced NI (attach form CA4139/CF383/CF380A)</t>
-  </si>
-  <si>
-    <t>Payroll Recognition ScenarioThree201718.xlsx</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH PAYROL RTI SCENRIO3 REPORT</t>
-  </si>
-  <si>
     <t>FirstNICatgoryChange</t>
   </si>
   <si>
@@ -489,9 +474,6 @@
     <t>May-2017</t>
   </si>
   <si>
-    <t>8161.32</t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
@@ -568,6 +550,9 @@
   </si>
   <si>
     <t>ExecuteQuery</t>
+  </si>
+  <si>
+    <t>12600.00</t>
   </si>
 </sst>
 </file>
@@ -991,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,7 +1004,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
@@ -1033,7 +1018,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>70</v>
@@ -1117,7 +1102,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>70</v>
@@ -1173,7 +1158,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>70</v>
@@ -1215,7 +1200,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>70</v>
@@ -1257,7 +1242,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>70</v>
@@ -1299,7 +1284,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>70</v>
@@ -1341,7 +1326,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>70</v>
@@ -1397,7 +1382,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>70</v>
@@ -1453,7 +1438,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>70</v>
@@ -1509,7 +1494,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>70</v>
@@ -1551,7 +1536,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>70</v>
@@ -1586,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1631,19 +1616,19 @@
     </row>
     <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -1661,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,10 +1716,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1742,23 +1727,23 @@
       <c r="E2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -1778,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1846,10 +1831,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1857,23 +1842,23 @@
       <c r="E2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -1893,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1950,13 +1935,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -1973,10 +1958,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1984,14 +1969,14 @@
       <c r="E2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>55</v>
@@ -2000,16 +1985,16 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>58</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -2027,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2096,10 +2081,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2107,14 +2092,14 @@
       <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>56</v>
@@ -2123,7 +2108,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -2143,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2210,10 +2195,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2221,23 +2206,23 @@
       <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -2257,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2314,13 +2299,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -2337,10 +2322,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2348,29 +2333,29 @@
       <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>60</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>61</v>
@@ -2391,8 +2376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2460,10 +2445,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2471,14 +2456,14 @@
       <c r="E2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>57</v>
@@ -2487,7 +2472,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -2508,7 +2493,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2520,7 +2505,9 @@
     <col min="6" max="6" customWidth="true" width="23.21875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="23.88671875" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="48.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2572,10 +2559,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2583,23 +2570,23 @@
       <c r="E2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -2619,8 +2606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2676,13 +2663,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -2699,10 +2686,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2710,32 +2697,32 @@
       <c r="E2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -2779,31 +2766,31 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -2817,28 +2804,28 @@
     </row>
     <row customHeight="1" ht="30" r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>8</v>
@@ -2864,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2935,10 +2922,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2946,23 +2933,23 @@
       <c r="E2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -2982,8 +2969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3049,10 +3036,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3060,23 +3047,23 @@
       <c r="E2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -3096,8 +3083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3150,13 +3137,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -3173,10 +3160,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3184,14 +3171,14 @@
       <c r="E2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>58</v>
@@ -3200,16 +3187,16 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -3228,7 +3215,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3298,10 +3285,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3309,23 +3296,23 @@
       <c r="E2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -3345,8 +3332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3413,10 +3400,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3424,23 +3411,23 @@
       <c r="E2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -3461,7 +3448,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3515,13 +3502,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -3538,10 +3525,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3549,32 +3536,32 @@
       <c r="E2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -3592,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3661,10 +3648,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3672,14 +3659,14 @@
       <c r="E2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>59</v>
@@ -3688,7 +3675,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -3708,8 +3695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3773,10 +3760,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3784,23 +3771,23 @@
       <c r="E2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -3820,8 +3807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3875,13 +3862,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -3898,10 +3885,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3909,32 +3896,32 @@
       <c r="E2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -3998,19 +3985,19 @@
     </row>
     <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -4030,7 +4017,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4074,19 +4061,19 @@
     </row>
     <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>159</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -4106,7 +4093,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4174,10 +4161,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -4185,23 +4172,23 @@
       <c r="E2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -4221,8 +4208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4287,10 +4274,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -4298,23 +4285,23 @@
       <c r="E2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -4334,8 +4321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4389,13 +4376,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -4412,10 +4399,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -4423,14 +4410,14 @@
       <c r="E2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>60</v>
@@ -4439,16 +4426,16 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -4511,19 +4498,19 @@
     </row>
     <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -4542,8 +4529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4611,25 +4598,25 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>81</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>61</v>
@@ -4638,7 +4625,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -4658,8 +4645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4671,6 +4658,7 @@
     <col min="6" max="6" customWidth="true" width="25.5546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4722,34 +4710,34 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>81</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -4769,8 +4757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4824,13 +4812,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -4847,43 +4835,43 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>81</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -4902,8 +4890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4971,34 +4959,34 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>80</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -5019,7 +5007,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5083,34 +5071,34 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>80</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -5130,8 +5118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5184,13 +5172,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -5207,43 +5195,43 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>80</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -5262,7 +5250,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5330,10 +5318,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>9</v>
@@ -5342,13 +5330,13 @@
         <v>51</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>52</v>
@@ -5445,10 +5433,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -5457,13 +5445,13 @@
         <v>51</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>53</v>
@@ -5547,13 +5535,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>2</v>
@@ -5570,10 +5558,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -5582,13 +5570,13 @@
         <v>51</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>74</v>
@@ -5600,7 +5588,7 @@
         <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>52</v>
@@ -5625,8 +5613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5694,34 +5682,34 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -5741,8 +5729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5810,25 +5798,25 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>54</v>
@@ -5837,7 +5825,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -5857,8 +5845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5913,13 +5901,13 @@
         <v>28</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -5936,37 +5924,37 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
XML Files created for RTI Scenarios
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
@@ -4,55 +4,55 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2376" windowWidth="9552" windowHeight="3564" firstSheet="28" activeTab="28"/>
+    <workbookView activeTab="28" firstSheet="28" windowHeight="3564" windowWidth="9552" xWindow="0" yWindow="2376"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
-    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
-    <sheet name="ProcessPayrollForMay" sheetId="16" r:id="rId7"/>
-    <sheet name="ProcessFinalPayrollForMay" sheetId="17" r:id="rId8"/>
-    <sheet name="TestMayReports" sheetId="18" r:id="rId9"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="51" r:id="rId10"/>
-    <sheet name="ProcessPayrollForJune" sheetId="19" r:id="rId11"/>
-    <sheet name="ProcessFinalPayrollForJune" sheetId="50" r:id="rId12"/>
-    <sheet name="TestJuneReports" sheetId="20" r:id="rId13"/>
-    <sheet name="ProcessPayrollForJuly" sheetId="22" r:id="rId14"/>
-    <sheet name="ProcessFinalPayrollForJuly" sheetId="52" r:id="rId15"/>
-    <sheet name="TestJulyReports" sheetId="23" r:id="rId16"/>
-    <sheet name="ProcessPayrollForAug" sheetId="25" r:id="rId17"/>
-    <sheet name="ProcessFinalPayrollForAug" sheetId="53" r:id="rId18"/>
-    <sheet name="TestAugReports" sheetId="26" r:id="rId19"/>
-    <sheet name="ProcessPayrollForSep" sheetId="28" r:id="rId20"/>
-    <sheet name="ProcessFinalPayrollForSep" sheetId="54" r:id="rId21"/>
-    <sheet name="TestSepReports" sheetId="29" r:id="rId22"/>
-    <sheet name="ProcessPayrollForOct" sheetId="31" r:id="rId23"/>
-    <sheet name="ProcessFinalPayrollForOct" sheetId="55" r:id="rId24"/>
-    <sheet name="TestOctReports" sheetId="32" r:id="rId25"/>
-    <sheet name="ProcessPayrollForNov" sheetId="34" r:id="rId26"/>
-    <sheet name="ProcessFinalPayrollForNov" sheetId="56" r:id="rId27"/>
-    <sheet name="TestNovReports" sheetId="35" r:id="rId28"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="36" r:id="rId29"/>
-    <sheet name="ProcessPayrollForDec" sheetId="37" r:id="rId30"/>
-    <sheet name="ProcessFinalPayrollForDec" sheetId="57" r:id="rId31"/>
-    <sheet name="TestDecReports" sheetId="38" r:id="rId32"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="39" r:id="rId33"/>
-    <sheet name="ProcessPayrollForJan" sheetId="40" r:id="rId34"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="58" r:id="rId35"/>
-    <sheet name="TestJanReports" sheetId="41" r:id="rId36"/>
-    <sheet name="ProcessPayrollForFeb" sheetId="43" r:id="rId37"/>
-    <sheet name="ProcessFinalPayrollForFeb" sheetId="59" r:id="rId38"/>
-    <sheet name="TestFebReports" sheetId="44" r:id="rId39"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
+    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
+    <sheet name="ProcessPayrollForMay" r:id="rId7" sheetId="16"/>
+    <sheet name="ProcessFinalPayrollForMay" r:id="rId8" sheetId="17"/>
+    <sheet name="TestMayReports" r:id="rId9" sheetId="18"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId10" sheetId="51"/>
+    <sheet name="ProcessPayrollForJune" r:id="rId11" sheetId="19"/>
+    <sheet name="ProcessFinalPayrollForJune" r:id="rId12" sheetId="50"/>
+    <sheet name="TestJuneReports" r:id="rId13" sheetId="20"/>
+    <sheet name="ProcessPayrollForJuly" r:id="rId14" sheetId="22"/>
+    <sheet name="ProcessFinalPayrollForJuly" r:id="rId15" sheetId="52"/>
+    <sheet name="TestJulyReports" r:id="rId16" sheetId="23"/>
+    <sheet name="ProcessPayrollForAug" r:id="rId17" sheetId="25"/>
+    <sheet name="ProcessFinalPayrollForAug" r:id="rId18" sheetId="53"/>
+    <sheet name="TestAugReports" r:id="rId19" sheetId="26"/>
+    <sheet name="ProcessPayrollForSep" r:id="rId20" sheetId="28"/>
+    <sheet name="ProcessFinalPayrollForSep" r:id="rId21" sheetId="54"/>
+    <sheet name="TestSepReports" r:id="rId22" sheetId="29"/>
+    <sheet name="ProcessPayrollForOct" r:id="rId23" sheetId="31"/>
+    <sheet name="ProcessFinalPayrollForOct" r:id="rId24" sheetId="55"/>
+    <sheet name="TestOctReports" r:id="rId25" sheetId="32"/>
+    <sheet name="ProcessPayrollForNov" r:id="rId26" sheetId="34"/>
+    <sheet name="ProcessFinalPayrollForNov" r:id="rId27" sheetId="56"/>
+    <sheet name="TestNovReports" r:id="rId28" sheetId="35"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId29" sheetId="36"/>
+    <sheet name="ProcessPayrollForDec" r:id="rId30" sheetId="37"/>
+    <sheet name="ProcessFinalPayrollForDec" r:id="rId31" sheetId="57"/>
+    <sheet name="TestDecReports" r:id="rId32" sheetId="38"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId33" sheetId="39"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId34" sheetId="40"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId35" sheetId="58"/>
+    <sheet name="TestJanReports" r:id="rId36" sheetId="41"/>
+    <sheet name="ProcessPayrollForFeb" r:id="rId37" sheetId="43"/>
+    <sheet name="ProcessFinalPayrollForFeb" r:id="rId38" sheetId="59"/>
+    <sheet name="TestFebReports" r:id="rId39" sheetId="44"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="164">
   <si>
     <t>TC</t>
   </si>
@@ -550,6 +550,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,66 +610,66 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -682,10 +683,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -843,7 +844,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -852,13 +853,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -868,7 +869,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -877,7 +878,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -886,7 +887,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -896,12 +897,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -932,7 +933,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -951,7 +952,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -963,7 +964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -972,10 +973,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1553,12 +1554,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1567,12 +1568,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1604,7 +1605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>142</v>
       </c>
@@ -1628,12 +1629,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -1642,19 +1643,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="51.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.88671875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1701,7 +1702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -1743,14 +1744,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -1759,17 +1760,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="49.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="49.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1816,7 +1817,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -1858,14 +1859,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -1874,23 +1875,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.5546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.5546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1943,7 +1944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -1992,14 +1993,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -2008,18 +2009,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2066,7 +2067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -2108,14 +2109,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -2124,16 +2125,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="52.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="52.77734375" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2180,7 +2181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -2222,14 +2223,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
@@ -2238,23 +2239,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.77734375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.77734375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.88671875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="5.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="5.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -2356,14 +2357,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -2372,18 +2373,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="40.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="53.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="53.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2430,7 +2431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -2472,14 +2473,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -2488,16 +2489,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2544,7 +2545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -2586,14 +2587,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -2602,23 +2603,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.21875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.44140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.21875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.21875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -2720,14 +2721,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2736,19 +2737,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.21875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.21875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -2792,7 +2793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="30" r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>142</v>
       </c>
@@ -2832,13 +2833,13 @@
       <c r="O2" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2847,20 +2848,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.21875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.77734375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.21875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2907,7 +2908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -2949,14 +2950,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2965,16 +2966,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3021,7 +3022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -3063,14 +3064,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3079,20 +3080,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3145,7 +3146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -3194,14 +3195,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -3210,20 +3211,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="52.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.21875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.21875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="52.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.21875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3270,7 +3271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -3312,14 +3313,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -3328,17 +3329,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.77734375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3385,7 +3386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -3427,14 +3428,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -3443,21 +3444,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="23.77734375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3510,7 +3511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -3559,14 +3560,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -3575,18 +3576,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3633,7 +3634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -3675,14 +3676,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3691,14 +3692,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3745,7 +3746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -3787,14 +3788,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -3803,21 +3804,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -3919,14 +3920,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3935,13 +3936,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3973,7 +3974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>142</v>
       </c>
@@ -3997,13 +3998,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4012,12 +4013,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4049,7 +4050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>142</v>
       </c>
@@ -4073,13 +4074,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -4088,18 +4089,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.44140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4146,7 +4147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -4188,14 +4189,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -4204,15 +4205,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.77734375" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4259,7 +4260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -4301,14 +4302,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -4317,21 +4318,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -4433,14 +4434,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4449,12 +4450,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="47.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4486,7 +4487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>142</v>
       </c>
@@ -4510,13 +4511,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -4525,18 +4526,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4583,7 +4584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -4625,14 +4626,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -4641,14 +4642,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4695,7 +4696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -4737,14 +4738,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -4753,21 +4754,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -4869,15 +4870,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -4886,18 +4887,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4944,7 +4945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -4986,14 +4987,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -5002,14 +5003,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5056,7 +5057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -5098,14 +5099,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -5114,20 +5115,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5180,7 +5181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -5229,14 +5230,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -5245,18 +5246,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5303,7 +5304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="16" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>71</v>
       </c>
@@ -5343,15 +5344,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -5360,18 +5361,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.21875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5418,7 +5419,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -5458,14 +5459,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -5474,23 +5475,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="18.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="1" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -5543,7 +5544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -5592,15 +5593,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -5609,18 +5610,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.77734375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5667,7 +5668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -5709,14 +5710,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -5725,18 +5726,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.77734375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5783,7 +5784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -5825,14 +5826,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -5841,22 +5842,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5909,7 +5910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
@@ -5958,9 +5959,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated RTI Scenario1,2,3 and 4
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
@@ -4,55 +4,55 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="28" firstSheet="28" windowHeight="3564" windowWidth="9552" xWindow="0" yWindow="2376"/>
+    <workbookView xWindow="0" yWindow="2376" windowWidth="9552" windowHeight="3564" firstSheet="30" activeTab="32"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
-    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
-    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
-    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
-    <sheet name="ProcessPayrollForMay" r:id="rId7" sheetId="16"/>
-    <sheet name="ProcessFinalPayrollForMay" r:id="rId8" sheetId="17"/>
-    <sheet name="TestMayReports" r:id="rId9" sheetId="18"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId10" sheetId="51"/>
-    <sheet name="ProcessPayrollForJune" r:id="rId11" sheetId="19"/>
-    <sheet name="ProcessFinalPayrollForJune" r:id="rId12" sheetId="50"/>
-    <sheet name="TestJuneReports" r:id="rId13" sheetId="20"/>
-    <sheet name="ProcessPayrollForJuly" r:id="rId14" sheetId="22"/>
-    <sheet name="ProcessFinalPayrollForJuly" r:id="rId15" sheetId="52"/>
-    <sheet name="TestJulyReports" r:id="rId16" sheetId="23"/>
-    <sheet name="ProcessPayrollForAug" r:id="rId17" sheetId="25"/>
-    <sheet name="ProcessFinalPayrollForAug" r:id="rId18" sheetId="53"/>
-    <sheet name="TestAugReports" r:id="rId19" sheetId="26"/>
-    <sheet name="ProcessPayrollForSep" r:id="rId20" sheetId="28"/>
-    <sheet name="ProcessFinalPayrollForSep" r:id="rId21" sheetId="54"/>
-    <sheet name="TestSepReports" r:id="rId22" sheetId="29"/>
-    <sheet name="ProcessPayrollForOct" r:id="rId23" sheetId="31"/>
-    <sheet name="ProcessFinalPayrollForOct" r:id="rId24" sheetId="55"/>
-    <sheet name="TestOctReports" r:id="rId25" sheetId="32"/>
-    <sheet name="ProcessPayrollForNov" r:id="rId26" sheetId="34"/>
-    <sheet name="ProcessFinalPayrollForNov" r:id="rId27" sheetId="56"/>
-    <sheet name="TestNovReports" r:id="rId28" sheetId="35"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId29" sheetId="36"/>
-    <sheet name="ProcessPayrollForDec" r:id="rId30" sheetId="37"/>
-    <sheet name="ProcessFinalPayrollForDec" r:id="rId31" sheetId="57"/>
-    <sheet name="TestDecReports" r:id="rId32" sheetId="38"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId33" sheetId="39"/>
-    <sheet name="ProcessPayrollForJan" r:id="rId34" sheetId="40"/>
-    <sheet name="ProcessFinalPayrollForJan" r:id="rId35" sheetId="58"/>
-    <sheet name="TestJanReports" r:id="rId36" sheetId="41"/>
-    <sheet name="ProcessPayrollForFeb" r:id="rId37" sheetId="43"/>
-    <sheet name="ProcessFinalPayrollForFeb" r:id="rId38" sheetId="59"/>
-    <sheet name="TestFebReports" r:id="rId39" sheetId="44"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
+    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
+    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
+    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
+    <sheet name="ProcessPayrollForMay" sheetId="16" r:id="rId7"/>
+    <sheet name="ProcessFinalPayrollForMay" sheetId="17" r:id="rId8"/>
+    <sheet name="TestMayReports" sheetId="18" r:id="rId9"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="51" r:id="rId10"/>
+    <sheet name="ProcessPayrollForJune" sheetId="19" r:id="rId11"/>
+    <sheet name="ProcessFinalPayrollForJune" sheetId="50" r:id="rId12"/>
+    <sheet name="TestJuneReports" sheetId="20" r:id="rId13"/>
+    <sheet name="ProcessPayrollForJuly" sheetId="22" r:id="rId14"/>
+    <sheet name="ProcessFinalPayrollForJuly" sheetId="52" r:id="rId15"/>
+    <sheet name="TestJulyReports" sheetId="23" r:id="rId16"/>
+    <sheet name="ProcessPayrollForAug" sheetId="25" r:id="rId17"/>
+    <sheet name="ProcessFinalPayrollForAug" sheetId="53" r:id="rId18"/>
+    <sheet name="TestAugReports" sheetId="26" r:id="rId19"/>
+    <sheet name="ProcessPayrollForSep" sheetId="28" r:id="rId20"/>
+    <sheet name="ProcessFinalPayrollForSep" sheetId="54" r:id="rId21"/>
+    <sheet name="TestSepReports" sheetId="29" r:id="rId22"/>
+    <sheet name="ProcessPayrollForOct" sheetId="31" r:id="rId23"/>
+    <sheet name="ProcessFinalPayrollForOct" sheetId="55" r:id="rId24"/>
+    <sheet name="TestOctReports" sheetId="32" r:id="rId25"/>
+    <sheet name="ProcessPayrollForNov" sheetId="34" r:id="rId26"/>
+    <sheet name="ProcessFinalPayrollForNov" sheetId="56" r:id="rId27"/>
+    <sheet name="TestNovReports" sheetId="35" r:id="rId28"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="36" r:id="rId29"/>
+    <sheet name="ProcessPayrollForDec" sheetId="37" r:id="rId30"/>
+    <sheet name="ProcessFinalPayrollForDec" sheetId="57" r:id="rId31"/>
+    <sheet name="TestDecReports" sheetId="38" r:id="rId32"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="39" r:id="rId33"/>
+    <sheet name="ProcessPayrollForJan" sheetId="40" r:id="rId34"/>
+    <sheet name="ProcessFinalPayrollForJan" sheetId="58" r:id="rId35"/>
+    <sheet name="TestJanReports" sheetId="41" r:id="rId36"/>
+    <sheet name="ProcessPayrollForFeb" sheetId="43" r:id="rId37"/>
+    <sheet name="ProcessFinalPayrollForFeb" sheetId="59" r:id="rId38"/>
+    <sheet name="TestFebReports" sheetId="44" r:id="rId39"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="164">
   <si>
     <t>TC</t>
   </si>
@@ -267,9 +267,6 @@
     <t>UpdteTaxCodeAndAnualSalaryM1</t>
   </si>
   <si>
-    <t>DONT TOUCH AUTO EMPLR HMRC RECNTION</t>
-  </si>
-  <si>
     <t>ProcessFinalPayrollForApril</t>
   </si>
   <si>
@@ -432,9 +429,6 @@
     <t>38</t>
   </si>
   <si>
-    <t>Monthly_RTIPayroll</t>
-  </si>
-  <si>
     <t>AddressFirstLine</t>
   </si>
   <si>
@@ -544,14 +538,19 @@
   </si>
   <si>
     <t>360</t>
+  </si>
+  <si>
+    <t>DONT TOUCH AUTO HMRCS4 EMPLOYER</t>
+  </si>
+  <si>
+    <t>HMRCS4_Payroll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,14 +562,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -609,67 +600,62 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -683,10 +669,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -844,7 +830,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -853,13 +839,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -869,7 +855,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -878,7 +864,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -887,7 +873,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -897,12 +883,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -933,7 +919,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -952,7 +938,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -964,7 +950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -973,10 +959,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -995,7 +981,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>69</v>
@@ -1009,7 +995,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>69</v>
@@ -1051,7 +1037,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>69</v>
@@ -1065,7 +1051,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>69</v>
@@ -1093,7 +1079,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>69</v>
@@ -1149,7 +1135,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>69</v>
@@ -1191,7 +1177,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>69</v>
@@ -1233,7 +1219,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>69</v>
@@ -1275,7 +1261,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>69</v>
@@ -1317,7 +1303,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>69</v>
@@ -1373,7 +1359,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>69</v>
@@ -1429,7 +1415,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>69</v>
@@ -1485,7 +1471,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>69</v>
@@ -1527,7 +1513,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>69</v>
@@ -1554,12 +1540,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1568,12 +1554,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1605,21 +1591,21 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>148</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -1629,33 +1615,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="31.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="28.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="1" max="1" width="41.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="51.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.88671875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1702,15 +1688,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1718,17 +1704,17 @@
       <c r="E2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -1744,33 +1730,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="49.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="1" max="1" width="42.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="49.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1817,15 +1803,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1833,17 +1819,17 @@
       <c r="E2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -1859,39 +1845,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="42.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="22.6640625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="6.5546875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="1" max="1" width="41.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="42.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="6.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1926,13 +1912,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -1944,15 +1930,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1960,14 +1946,14 @@
       <c r="E2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>54</v>
@@ -1982,10 +1968,10 @@
         <v>57</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -1993,34 +1979,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.77734375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.21875" collapsed="true"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2067,15 +2053,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2083,14 +2069,14 @@
       <c r="E2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>55</v>
@@ -2109,32 +2095,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="52.77734375" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.44140625" collapsed="true"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="52.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2181,15 +2167,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2197,17 +2183,17 @@
       <c r="E2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -2223,39 +2209,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="21.77734375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="9.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="5.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="21.77734375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="5.88671875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="5.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2290,13 +2276,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -2308,15 +2294,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2324,17 +2310,17 @@
       <c r="E2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -2346,7 +2332,7 @@
         <v>59</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>60</v>
@@ -2357,34 +2343,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="40.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="39.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="53.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="40.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="53.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2431,15 +2417,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2447,14 +2433,14 @@
       <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>56</v>
@@ -2473,32 +2459,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="23.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="48.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2545,15 +2531,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2561,17 +2547,17 @@
       <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -2587,39 +2573,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="26.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="6.21875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="6.6640625" collapsed="true"/>
+    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="22.21875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.44140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="6.21875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="6.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2654,13 +2640,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -2672,15 +2658,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2688,17 +2674,17 @@
       <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -2707,13 +2693,13 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -2721,14 +2707,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2737,19 +2723,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="8.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="9.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="6.21875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="1" max="1" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.21875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -2757,31 +2743,31 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -2793,30 +2779,30 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="G2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>146</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>8</v>
@@ -2833,35 +2819,35 @@
       <c r="O2" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.21875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="6.5546875" collapsed="true"/>
+    <col min="1" max="1" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.21875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.77734375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2908,15 +2894,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -2924,17 +2910,17 @@
       <c r="E2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -2950,32 +2936,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3022,15 +3008,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3038,17 +3024,17 @@
       <c r="E2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -3064,36 +3050,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="38.77734375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="21.44140625" collapsed="true"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="38.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="21.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3128,13 +3114,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -3146,15 +3132,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3162,14 +3148,14 @@
       <c r="E2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>57</v>
@@ -3181,13 +3167,13 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -3195,36 +3181,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="52.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.21875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="1" max="1" width="32.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="52.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.21875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.21875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3271,15 +3257,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3287,17 +3273,17 @@
       <c r="E2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -3313,33 +3299,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="48.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3386,15 +3372,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3402,17 +3388,17 @@
       <c r="E2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -3428,37 +3414,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="23.77734375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="23.77734375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3493,13 +3479,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -3511,15 +3497,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3527,17 +3513,17 @@
       <c r="E2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -3546,13 +3532,13 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -3560,34 +3546,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="48.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3634,15 +3620,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3650,14 +3636,14 @@
       <c r="E2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>58</v>
@@ -3676,30 +3662,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.77734375" collapsed="true"/>
+    <col min="1" max="1" width="39.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="47.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3746,15 +3732,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3762,17 +3748,17 @@
       <c r="E2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -3788,37 +3774,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="47.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="22" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3853,13 +3839,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -3871,15 +3857,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -3887,17 +3873,17 @@
       <c r="E2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -3906,13 +3892,13 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -3920,29 +3906,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="8.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="1" width="48.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3974,21 +3960,21 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>148</v>
+        <v>160</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -3998,27 +3984,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="1" max="1" width="32.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4050,21 +4036,21 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="E2" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -4074,33 +4060,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.44140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.44140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4147,15 +4133,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -4163,23 +4149,23 @@
       <c r="E2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -4189,31 +4175,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.77734375" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="47.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4260,15 +4246,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -4276,17 +4262,17 @@
       <c r="E2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -4302,37 +4288,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="1" max="1" width="31.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="46.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="24" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4367,13 +4353,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -4385,15 +4371,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -4401,14 +4387,14 @@
       <c r="E2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>59</v>
@@ -4420,13 +4406,13 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -4434,28 +4420,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="47.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="1" max="2" width="47.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4487,21 +4473,21 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>148</v>
+        <v>160</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>9</v>
@@ -4511,33 +4497,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.21875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="46.44140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4584,30 +4570,30 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>60</v>
@@ -4626,30 +4612,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="47.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4696,33 +4682,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -4738,37 +4724,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="24.33203125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4803,13 +4789,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -4821,33 +4807,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -4856,13 +4842,13 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -4870,35 +4856,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="40.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="1" max="1" width="40.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="47.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4945,33 +4931,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -4987,30 +4973,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.77734375" collapsed="true"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5057,33 +5043,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -5099,36 +5085,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.21875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="24.77734375" collapsed="true"/>
+    <col min="1" max="1" width="41.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="48" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="24.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5163,13 +5149,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -5181,33 +5167,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -5216,13 +5202,13 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
@@ -5230,34 +5216,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="1" max="1" width="40" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="46.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5304,75 +5290,72 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>142</v>
+    <row r="2" spans="1:14" s="14" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
-  </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="28.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="1" max="1" width="32.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.21875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5419,15 +5402,15 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -5436,13 +5419,13 @@
         <v>50</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>52</v>
@@ -5459,100 +5442,100 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="1" max="1" width="26.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="47.44140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="28.8" r="1" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="9" t="s">
+      <c r="P1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -5561,16 +5544,16 @@
         <v>50</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -5579,7 +5562,7 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>51</v>
@@ -5593,35 +5576,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="46" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5668,33 +5651,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="I2" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -5710,34 +5693,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="48.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.88671875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5784,30 +5767,30 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>53</v>
@@ -5826,38 +5809,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="27" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5892,13 +5875,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -5910,33 +5893,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>23</v>
@@ -5945,7 +5928,7 @@
         <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>54</v>
@@ -5959,9 +5942,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Comitting base class with new QA Org changes
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFour201718.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="32" firstSheet="30" windowHeight="3564" windowWidth="9552" xWindow="0" yWindow="2376"/>
+    <workbookView activeTab="22" firstSheet="19" windowHeight="3570" windowWidth="9555" xWindow="0" yWindow="2370"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -47,12 +52,12 @@
     <sheet name="ProcessFinalPayrollForFeb" r:id="rId38" sheetId="59"/>
     <sheet name="TestFebReports" r:id="rId39" sheetId="44"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="164">
   <si>
     <t>TC</t>
   </si>
@@ -549,7 +554,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -661,6 +666,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -708,7 +716,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -741,9 +749,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -776,6 +801,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -958,15 +1000,15 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -980,7 +1022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -994,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -1008,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1022,7 +1064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1036,7 +1078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -1050,7 +1092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1064,7 +1106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1078,7 +1120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -1092,7 +1134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1106,7 +1148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1120,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1134,7 +1176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -1148,7 +1190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1162,7 +1204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1176,7 +1218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1190,7 +1232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1204,7 +1246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1218,7 +1260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -1232,7 +1274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1246,7 +1288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1260,7 +1302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -1274,7 +1316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1288,7 +1330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1302,7 +1344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1316,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1330,7 +1372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1344,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1358,7 +1400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -1372,7 +1414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1386,7 +1428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1400,7 +1442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1414,7 +1456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -1428,7 +1470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -1442,7 +1484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1456,7 +1498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1470,7 +1512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1484,7 +1526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -1498,7 +1540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -1512,7 +1554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -1526,7 +1568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1553,17 +1595,17 @@
       <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1592,7 +1634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>140</v>
       </c>
@@ -1628,24 +1670,24 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="31.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="28.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="51.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1689,7 +1731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -1745,22 +1787,22 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="49.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="49.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1804,7 +1846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -1860,25 +1902,25 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="42.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.7109375" collapsed="true"/>
     <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="6.5546875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1931,7 +1973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -1994,23 +2036,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.77734375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.5546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.5703125" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2054,7 +2096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -2110,21 +2152,21 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="52.77734375" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.44140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="52.7109375" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2168,7 +2210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -2224,25 +2266,25 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="21.77734375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="9.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="5.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="5.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2295,7 +2337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -2358,23 +2400,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="40.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="39.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="53.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="53.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2418,7 +2460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -2474,21 +2516,21 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="23.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2532,7 +2574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -2588,25 +2630,25 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="26.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="45.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="6.21875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="6.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2659,7 +2701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -2722,24 +2764,24 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="8.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="9.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="6.21875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2780,7 +2822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="30" r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>140</v>
       </c>
@@ -2833,25 +2875,25 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.21875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="6.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2895,7 +2937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -2948,24 +2990,24 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
     <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3009,7 +3051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -3065,22 +3107,22 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="38.77734375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="21.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3133,7 +3175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -3192,29 +3234,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.21875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="52.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.21875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="52.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3258,7 +3300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -3314,22 +3356,22 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3373,7 +3415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -3429,23 +3471,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="23.77734375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3498,7 +3540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -3561,23 +3603,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.140625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3621,7 +3663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -3677,19 +3719,19 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.7109375" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3733,7 +3775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -3789,23 +3831,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
     <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3858,7 +3900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -3921,18 +3963,18 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="40.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="8.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3961,7 +4003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="40.9" r="2" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>140</v>
       </c>
@@ -3998,17 +4040,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.5546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4037,7 +4079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>140</v>
       </c>
@@ -4074,23 +4116,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.44140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4134,7 +4176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -4190,20 +4232,20 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.77734375" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4247,7 +4289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -4303,23 +4345,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5703125" collapsed="true"/>
     <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4372,7 +4414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -4431,21 +4473,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="47.6640625" collapsed="true"/>
+    <col min="1" max="2" customWidth="true" width="47.7109375" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4474,7 +4516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="40.9" r="2" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>140</v>
       </c>
@@ -4511,23 +4553,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.21875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4571,7 +4613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -4627,19 +4669,19 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.5703125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4683,7 +4725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -4739,23 +4781,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4808,7 +4850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -4872,23 +4914,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="40.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4932,7 +4974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -4988,19 +5030,19 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5044,7 +5086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -5100,22 +5142,22 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.21875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.140625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="48.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="24.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5168,7 +5210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -5231,23 +5273,23 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="40.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5291,7 +5333,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -5343,23 +5385,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="28.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5403,7 +5445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -5457,25 +5499,25 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.21875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="47.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.42578125" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="28.8" r="1" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="30" r="1" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
@@ -5528,7 +5570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -5592,23 +5634,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="46.0" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
     <col min="11" max="11" customWidth="true" width="24.0" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5652,7 +5694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -5708,23 +5750,23 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="48.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5768,7 +5810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>
@@ -5824,24 +5866,24 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.7109375" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -5894,7 +5936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>162</v>
       </c>

</xml_diff>